<commit_message>
adding ganttchart + report
</commit_message>
<xml_diff>
--- a/Compute.Documents/Schedule/GanttWorkflow.xlsx
+++ b/Compute.Documents/Schedule/GanttWorkflow.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Plan</t>
   </si>
@@ -59,84 +59,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -224,6 +146,36 @@
   </si>
   <si>
     <t>Honours Project</t>
+  </si>
+  <si>
+    <t>Embed V8 Version 5.5.5</t>
+  </si>
+  <si>
+    <t>Implement CommonJs Modules</t>
+  </si>
+  <si>
+    <t>OpenGL Bindings</t>
+  </si>
+  <si>
+    <t>OpenCL Bindings</t>
+  </si>
+  <si>
+    <t>Core Modules (Http, Console, Timer)</t>
+  </si>
+  <si>
+    <t>Relevant Reading</t>
+  </si>
+  <si>
+    <t>Interim Report</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Basic Demo</t>
+  </si>
+  <si>
+    <t>Debugging &amp; Testing</t>
   </si>
 </sst>
 </file>
@@ -427,7 +379,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -481,9 +433,6 @@
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -502,7 +451,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -519,15 +468,6 @@
         <bottom style="thin">
           <color theme="7"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
         <vertical/>
         <horizontal/>
       </border>
@@ -953,16 +893,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ34"/>
+  <dimension ref="B2:AX40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.375" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
@@ -970,25 +910,25 @@
     <col min="9" max="28" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+    <row r="2" spans="2:50" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="2:50" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="I3" s="8" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -999,20 +939,20 @@
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="T3" s="11"/>
-      <c r="U3" s="19" t="s">
+      <c r="U3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -1020,28 +960,28 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:50" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:50" x14ac:dyDescent="0.3">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:69" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:50" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -1065,7 +1005,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1090,7 +1030,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1137,705 +1077,953 @@
       <c r="U8" s="3">
         <v>13</v>
       </c>
-      <c r="V8" s="3">
-        <v>14</v>
-      </c>
-      <c r="W8" s="3">
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+    </row>
+    <row r="9" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="X8" s="3">
-        <v>16</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>17</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>18</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>19</v>
-      </c>
-      <c r="AB8" s="3">
-        <v>20</v>
-      </c>
-      <c r="AC8" s="3">
-        <v>21</v>
-      </c>
-      <c r="AD8" s="3">
-        <v>22</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>23</v>
-      </c>
-      <c r="AF8" s="3">
-        <v>24</v>
-      </c>
-      <c r="AG8" s="3">
-        <v>25</v>
-      </c>
-      <c r="AH8" s="3">
-        <v>26</v>
-      </c>
-      <c r="AI8" s="3">
-        <v>27</v>
-      </c>
-      <c r="AJ8" s="3">
-        <v>28</v>
-      </c>
-      <c r="AK8" s="3">
-        <v>29</v>
-      </c>
-      <c r="AL8" s="3">
-        <v>30</v>
-      </c>
-      <c r="AM8" s="3">
-        <v>31</v>
-      </c>
-      <c r="AN8" s="3">
-        <v>32</v>
-      </c>
-      <c r="AO8" s="3">
-        <v>33</v>
-      </c>
-      <c r="AP8" s="3">
-        <v>34</v>
-      </c>
-      <c r="AQ8" s="3">
-        <v>35</v>
-      </c>
-      <c r="AR8" s="3">
-        <v>36</v>
-      </c>
-      <c r="AS8" s="3">
-        <v>37</v>
-      </c>
-      <c r="AT8" s="3">
-        <v>38</v>
-      </c>
-      <c r="AU8" s="3">
-        <v>39</v>
-      </c>
-      <c r="AV8" s="3">
-        <v>40</v>
-      </c>
-      <c r="AW8" s="3">
-        <v>41</v>
-      </c>
-      <c r="AX8" s="3">
-        <v>42</v>
-      </c>
-      <c r="AY8" s="3">
-        <v>43</v>
-      </c>
-      <c r="AZ8" s="3">
-        <v>44</v>
-      </c>
-      <c r="BA8" s="3">
-        <v>45</v>
-      </c>
-      <c r="BB8" s="3">
-        <v>46</v>
-      </c>
-      <c r="BC8" s="3">
-        <v>47</v>
-      </c>
-      <c r="BD8" s="3">
-        <v>48</v>
-      </c>
-      <c r="BE8" s="3">
-        <v>49</v>
-      </c>
-      <c r="BF8" s="3">
-        <v>50</v>
-      </c>
-      <c r="BG8" s="3">
-        <v>51</v>
-      </c>
-      <c r="BH8" s="3">
-        <v>52</v>
-      </c>
-      <c r="BI8" s="3">
-        <v>53</v>
-      </c>
-      <c r="BJ8" s="3">
-        <v>54</v>
-      </c>
-      <c r="BK8" s="3">
-        <v>55</v>
-      </c>
-      <c r="BL8" s="3">
-        <v>56</v>
-      </c>
-      <c r="BM8" s="3">
-        <v>57</v>
-      </c>
-      <c r="BN8" s="3">
-        <v>58</v>
-      </c>
-      <c r="BO8" s="3">
-        <v>59</v>
-      </c>
-      <c r="BP8" s="3">
-        <v>60</v>
-      </c>
-      <c r="BQ8" s="1"/>
-    </row>
-    <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
-        <v>10</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
       </c>
       <c r="D9" s="16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="16">
         <v>1</v>
       </c>
       <c r="F9" s="16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="17">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+    </row>
+    <row r="10" spans="2:50" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C10" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E10" s="16">
         <v>1</v>
       </c>
       <c r="F10" s="16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G10" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+    </row>
+    <row r="11" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C11" s="16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" s="16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G11" s="17">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
+    </row>
+    <row r="12" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C12" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E12" s="16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F12" s="16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G12" s="17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+    </row>
+    <row r="13" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C13" s="16">
+        <v>3</v>
+      </c>
+      <c r="D13" s="16">
+        <v>3</v>
+      </c>
+      <c r="E13" s="16">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16">
         <v>4</v>
       </c>
-      <c r="D13" s="16">
+      <c r="G13" s="17">
+        <v>1</v>
+      </c>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+    </row>
+    <row r="14" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="16">
         <v>2</v>
       </c>
-      <c r="E13" s="16">
-        <v>4</v>
-      </c>
-      <c r="F13" s="16">
+      <c r="D14" s="16">
         <v>8</v>
       </c>
-      <c r="G13" s="17">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="16">
-        <v>4</v>
-      </c>
-      <c r="D14" s="16">
-        <v>3</v>
-      </c>
       <c r="E14" s="16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" s="16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G14" s="17">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+    </row>
+    <row r="15" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C15" s="16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" s="16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E15" s="16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F15" s="16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+    </row>
+    <row r="16" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C16" s="16">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D16" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16" s="16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G16" s="17">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+    </row>
+    <row r="17" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C17" s="16">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D17" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F17" s="16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G17" s="17">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+    </row>
+    <row r="18" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C18" s="16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D18" s="16">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E18" s="16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F18" s="16">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G18" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="18">
-        <v>6</v>
-      </c>
-      <c r="D19" s="16">
-        <v>1</v>
-      </c>
-      <c r="E19" s="16">
-        <v>5</v>
-      </c>
-      <c r="F19" s="16">
-        <v>8</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="16">
-        <v>9</v>
-      </c>
-      <c r="D20" s="16">
-        <v>3</v>
-      </c>
-      <c r="E20" s="16">
-        <v>9</v>
-      </c>
-      <c r="F20" s="16">
-        <v>3</v>
-      </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="16">
-        <v>9</v>
-      </c>
-      <c r="D21" s="16">
-        <v>6</v>
-      </c>
-      <c r="E21" s="16">
-        <v>9</v>
-      </c>
-      <c r="F21" s="16">
-        <v>7</v>
-      </c>
-      <c r="G21" s="17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="16">
-        <v>9</v>
-      </c>
-      <c r="D22" s="16">
-        <v>3</v>
-      </c>
-      <c r="E22" s="16">
-        <v>9</v>
-      </c>
-      <c r="F22" s="16">
-        <v>1</v>
-      </c>
-      <c r="G22" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="16">
-        <v>9</v>
-      </c>
-      <c r="D23" s="16">
-        <v>4</v>
-      </c>
-      <c r="E23" s="16">
-        <v>8</v>
-      </c>
-      <c r="F23" s="16">
-        <v>5</v>
-      </c>
-      <c r="G23" s="17">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="16">
-        <v>10</v>
-      </c>
-      <c r="D24" s="16">
-        <v>5</v>
-      </c>
-      <c r="E24" s="16">
-        <v>10</v>
-      </c>
-      <c r="F24" s="16">
-        <v>3</v>
-      </c>
-      <c r="G24" s="17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="16">
-        <v>11</v>
-      </c>
-      <c r="D25" s="16">
-        <v>2</v>
-      </c>
-      <c r="E25" s="16">
-        <v>11</v>
-      </c>
-      <c r="F25" s="16">
-        <v>5</v>
-      </c>
-      <c r="G25" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="16">
-        <v>12</v>
-      </c>
-      <c r="D26" s="16">
-        <v>6</v>
-      </c>
-      <c r="E26" s="16">
-        <v>12</v>
-      </c>
-      <c r="F26" s="16">
-        <v>7</v>
-      </c>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="16">
-        <v>12</v>
-      </c>
-      <c r="D27" s="16">
-        <v>1</v>
-      </c>
-      <c r="E27" s="16">
-        <v>12</v>
-      </c>
-      <c r="F27" s="16">
-        <v>5</v>
-      </c>
-      <c r="G27" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="16">
-        <v>14</v>
-      </c>
-      <c r="D28" s="16">
-        <v>5</v>
-      </c>
-      <c r="E28" s="16">
-        <v>14</v>
-      </c>
-      <c r="F28" s="16">
-        <v>6</v>
-      </c>
-      <c r="G28" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="16">
-        <v>14</v>
-      </c>
-      <c r="D29" s="16">
-        <v>8</v>
-      </c>
-      <c r="E29" s="16">
-        <v>14</v>
-      </c>
-      <c r="F29" s="16">
-        <v>2</v>
-      </c>
-      <c r="G29" s="17">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="16">
-        <v>14</v>
-      </c>
-      <c r="D30" s="16">
-        <v>7</v>
-      </c>
-      <c r="E30" s="16">
-        <v>14</v>
-      </c>
-      <c r="F30" s="16">
-        <v>3</v>
-      </c>
-      <c r="G30" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="16">
-        <v>15</v>
-      </c>
-      <c r="D31" s="16">
-        <v>4</v>
-      </c>
-      <c r="E31" s="16">
-        <v>15</v>
-      </c>
-      <c r="F31" s="16">
-        <v>8</v>
-      </c>
-      <c r="G31" s="17">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="16">
-        <v>15</v>
-      </c>
-      <c r="D32" s="16">
-        <v>5</v>
-      </c>
-      <c r="E32" s="16">
-        <v>15</v>
-      </c>
-      <c r="F32" s="16">
-        <v>3</v>
-      </c>
-      <c r="G32" s="17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="16">
-        <v>15</v>
-      </c>
-      <c r="D33" s="16">
-        <v>8</v>
-      </c>
-      <c r="E33" s="16">
-        <v>15</v>
-      </c>
-      <c r="F33" s="16">
-        <v>5</v>
-      </c>
-      <c r="G33" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="16">
-        <v>16</v>
-      </c>
-      <c r="D34" s="16">
-        <v>28</v>
-      </c>
-      <c r="E34" s="16">
-        <v>16</v>
-      </c>
-      <c r="F34" s="16">
-        <v>30</v>
-      </c>
-      <c r="G34" s="17">
-        <v>0.5</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+    </row>
+    <row r="19" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+    </row>
+    <row r="20" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+    </row>
+    <row r="21" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+    </row>
+    <row r="22" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+    </row>
+    <row r="23" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+      <c r="AB23"/>
+    </row>
+    <row r="24" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+      <c r="AB24"/>
+    </row>
+    <row r="25" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+    </row>
+    <row r="26" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+      <c r="AB26"/>
+    </row>
+    <row r="27" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
+      <c r="AB27"/>
+    </row>
+    <row r="28" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
+    </row>
+    <row r="29" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+      <c r="AB29"/>
+    </row>
+    <row r="30" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+      <c r="AB30"/>
+    </row>
+    <row r="31" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+      <c r="AB31"/>
+    </row>
+    <row r="32" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+    </row>
+    <row r="33" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+      <c r="AA33"/>
+      <c r="AB33"/>
+    </row>
+    <row r="34" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+    </row>
+    <row r="35" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+    </row>
+    <row r="36" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+    </row>
+    <row r="37" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+    </row>
+    <row r="38" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+    </row>
+    <row r="39" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+    </row>
+    <row r="40" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP34">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="I9:U18">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:BP35">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8:BP8">
+  <conditionalFormatting sqref="I8:U8">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>I$8=period_selected</formula>
     </cfRule>

</xml_diff>